<commit_message>
Update to CM file
</commit_message>
<xml_diff>
--- a/inst/extdata/Signatures.xlsx
+++ b/inst/extdata/Signatures.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10808"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10912"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/chineduanene/Documents/GitHub/Decosus/inst/extdata/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2CF4802F-3E40-0541-A540-400F9ECB7783}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DDF2D8B0-456F-2942-9E45-EBE0E98199DB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="880" yWindow="500" windowWidth="33520" windowHeight="21000" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="33600" windowHeight="21000" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Curated" sheetId="1" r:id="rId1"/>
@@ -37,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2011" uniqueCount="479">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2012" uniqueCount="479">
   <si>
     <t>Type</t>
   </si>
@@ -5211,8 +5211,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:E154"/>
   <sheetViews>
-    <sheetView zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
-      <selection activeCell="C123" sqref="C123:C124"/>
+    <sheetView tabSelected="1" topLeftCell="A91" zoomScale="125" zoomScaleNormal="80" workbookViewId="0">
+      <selection activeCell="F120" sqref="F120"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="10.83203125" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -5965,7 +5965,9 @@
       <c r="B64" s="2" t="s">
         <v>311</v>
       </c>
-      <c r="C64" s="2"/>
+      <c r="C64" s="2" t="s">
+        <v>312</v>
+      </c>
       <c r="D64" s="2" t="s">
         <v>312</v>
       </c>
@@ -7020,13 +7022,13 @@
     </row>
   </sheetData>
   <autoFilter ref="A1:D135" xr:uid="{48D8CAE7-6202-46D0-892E-92FC19BD528C}"/>
-  <conditionalFormatting sqref="C1:C6 C16:C114 C117:C1048576 C8:C14">
+  <conditionalFormatting sqref="C1:C6 C16:C63 C117:C1048576 C8:C14 C65:C114">
     <cfRule type="duplicateValues" dxfId="7" priority="3"/>
   </conditionalFormatting>
-  <conditionalFormatting sqref="C1:C6 C8:C114 C116:C1048576">
+  <conditionalFormatting sqref="C1:C6 C8:C63 C116:C1048576 C65:C114">
     <cfRule type="duplicateValues" dxfId="6" priority="2"/>
   </conditionalFormatting>
-  <conditionalFormatting sqref="C1:C1048576">
+  <conditionalFormatting sqref="C1:C63 C65:C1048576">
     <cfRule type="duplicateValues" dxfId="5" priority="1"/>
   </conditionalFormatting>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -7467,7 +7469,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{21267F1A-3001-4148-9909-E8C4D58FC8DD}">
   <dimension ref="A1:B92"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A49" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="H73" sqref="H73"/>
     </sheetView>
   </sheetViews>

</xml_diff>